<commit_message>
women data updated - sheet total everywhere
</commit_message>
<xml_diff>
--- a/data/women/W_2019_05_MCR.xlsx
+++ b/data/women/W_2019_05_MCR.xlsx
@@ -1,33 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzelenka\Documents\python_j\fencing\data\women\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C083A609-92B9-4E7A-B144-C6FBED895FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95643156-43EF-43C9-84F1-FB01DEB1C0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12048" yWindow="-15060" windowWidth="15228" windowHeight="13212" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1344" yWindow="-11052" windowWidth="23040" windowHeight="7716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="initiation" sheetId="1" r:id="rId1"/>
-    <sheet name="first_round" sheetId="2" r:id="rId2"/>
-    <sheet name="total_rank" sheetId="3" r:id="rId3"/>
-    <sheet name="pools" sheetId="4" r:id="rId4"/>
-    <sheet name="eliminations" sheetId="5" r:id="rId5"/>
+    <sheet name="total" sheetId="6" r:id="rId1"/>
+    <sheet name="initiation" sheetId="1" r:id="rId2"/>
+    <sheet name="first_round" sheetId="2" r:id="rId3"/>
+    <sheet name="total_rank" sheetId="3" r:id="rId4"/>
+    <sheet name="pools" sheetId="4" r:id="rId5"/>
+    <sheet name="eliminations" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">eliminations!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">first_round!$A$1:$M$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">initiation!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">pools!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">total_rank!$A$1:$H$1</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">first_round!#REF!</definedName>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">initiation!#REF!</definedName>
-    <definedName name="ExternalData_1" localSheetId="2" hidden="1">total_rank!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">eliminations!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">first_round!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">initiation!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">pools!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">total!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">total_rank!$A$1:$H$1</definedName>
+    <definedName name="ExternalData_1" localSheetId="2" hidden="1">first_round!#REF!</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">initiation!#REF!</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">total_rank!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -94,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2250" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -320,6 +322,9 @@
   <si>
     <t>Eliminace_2</t>
   </si>
+  <si>
+    <t>Percentil</t>
+  </si>
 </sst>
 </file>
 
@@ -390,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -422,6 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,11 +707,1708 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009EEB42-AF0B-4CD6-B9D9-CB19FB8E0451}">
+  <dimension ref="A1:Q31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1">
+        <v>37414</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="K2" s="5">
+        <v>16</v>
+      </c>
+      <c r="L2" s="5">
+        <v>23</v>
+      </c>
+      <c r="M2" s="5">
+        <v>-7</v>
+      </c>
+      <c r="N2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2">
+        <v>26</v>
+      </c>
+      <c r="P2">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="17">
+        <f>P2/MAX($P$2:$P$31)</f>
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1">
+        <v>37371</v>
+      </c>
+      <c r="I3" s="5">
+        <v>4</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="5">
+        <v>20</v>
+      </c>
+      <c r="L3" s="5">
+        <v>14</v>
+      </c>
+      <c r="M3" s="5">
+        <v>6</v>
+      </c>
+      <c r="N3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="17">
+        <f t="shared" ref="Q3:Q31" si="0">P3/MAX($P$2:$P$31)</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>36617</v>
+      </c>
+      <c r="I4" s="5">
+        <v>4</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="K4" s="5">
+        <v>20</v>
+      </c>
+      <c r="L4" s="5">
+        <v>15</v>
+      </c>
+      <c r="M4" s="5">
+        <v>5</v>
+      </c>
+      <c r="N4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="17">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1">
+        <v>29490</v>
+      </c>
+      <c r="I5" s="5">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K5" s="5">
+        <v>20</v>
+      </c>
+      <c r="L5" s="5">
+        <v>19</v>
+      </c>
+      <c r="M5" s="5">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5">
+        <v>13</v>
+      </c>
+      <c r="P5">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="17">
+        <f t="shared" si="0"/>
+        <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1">
+        <v>37189</v>
+      </c>
+      <c r="I6" s="5">
+        <v>3</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K6" s="5">
+        <v>21</v>
+      </c>
+      <c r="L6" s="5">
+        <v>17</v>
+      </c>
+      <c r="M6" s="5">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6">
+        <v>8</v>
+      </c>
+      <c r="P6">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="17">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>33</v>
+      </c>
+      <c r="H7" s="1">
+        <v>37903</v>
+      </c>
+      <c r="I7" s="5">
+        <v>2</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="K7" s="5">
+        <v>15</v>
+      </c>
+      <c r="L7" s="5">
+        <v>20</v>
+      </c>
+      <c r="M7" s="5">
+        <v>-5</v>
+      </c>
+      <c r="N7" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7">
+        <v>24</v>
+      </c>
+      <c r="P7">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="17">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>36213</v>
+      </c>
+      <c r="I8" s="5">
+        <v>3</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K8" s="5">
+        <v>22</v>
+      </c>
+      <c r="L8" s="5">
+        <v>19</v>
+      </c>
+      <c r="M8" s="5">
+        <v>3</v>
+      </c>
+      <c r="N8" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8">
+        <v>10</v>
+      </c>
+      <c r="P8">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="17">
+        <f t="shared" si="0"/>
+        <v>0.23333333333333334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1">
+        <v>33010</v>
+      </c>
+      <c r="I9" s="5">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K9" s="5">
+        <v>23</v>
+      </c>
+      <c r="L9" s="5">
+        <v>18</v>
+      </c>
+      <c r="M9" s="5">
+        <v>5</v>
+      </c>
+      <c r="N9" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9">
+        <v>5</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="17">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1">
+        <v>33437</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
+        <v>16</v>
+      </c>
+      <c r="L10" s="5">
+        <v>25</v>
+      </c>
+      <c r="M10" s="5">
+        <v>-9</v>
+      </c>
+      <c r="N10" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10">
+        <v>29</v>
+      </c>
+      <c r="P10">
+        <v>29</v>
+      </c>
+      <c r="Q10" s="17">
+        <f t="shared" si="0"/>
+        <v>0.96666666666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>23</v>
+      </c>
+      <c r="H11" s="1">
+        <v>37934</v>
+      </c>
+      <c r="I11" s="5">
+        <v>3</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K11" s="5">
+        <v>20</v>
+      </c>
+      <c r="L11" s="5">
+        <v>20</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O11">
+        <v>14</v>
+      </c>
+      <c r="P11">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="17">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>21</v>
+      </c>
+      <c r="H12" s="1">
+        <v>35537</v>
+      </c>
+      <c r="I12" s="5">
+        <v>2</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="K12" s="5">
+        <v>18</v>
+      </c>
+      <c r="L12" s="5">
+        <v>20</v>
+      </c>
+      <c r="M12" s="5">
+        <v>-2</v>
+      </c>
+      <c r="N12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12">
+        <v>21</v>
+      </c>
+      <c r="P12">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="17">
+        <f t="shared" si="0"/>
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>14</v>
+      </c>
+      <c r="H13" s="1">
+        <v>34628</v>
+      </c>
+      <c r="I13" s="5">
+        <v>4</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="5">
+        <v>23</v>
+      </c>
+      <c r="L13" s="5">
+        <v>20</v>
+      </c>
+      <c r="M13" s="5">
+        <v>3</v>
+      </c>
+      <c r="N13" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="17">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14" s="1">
+        <v>36590</v>
+      </c>
+      <c r="I14" s="5">
+        <v>3</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K14" s="5">
+        <v>22</v>
+      </c>
+      <c r="L14" s="5">
+        <v>19</v>
+      </c>
+      <c r="M14" s="5">
+        <v>3</v>
+      </c>
+      <c r="N14" t="s">
+        <v>51</v>
+      </c>
+      <c r="O14">
+        <v>10</v>
+      </c>
+      <c r="P14">
+        <v>17</v>
+      </c>
+      <c r="Q14" s="17">
+        <f t="shared" si="0"/>
+        <v>0.56666666666666665</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15" s="1">
+        <v>36590</v>
+      </c>
+      <c r="I15" s="5">
+        <v>3</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K15" s="5">
+        <v>20</v>
+      </c>
+      <c r="L15" s="5">
+        <v>15</v>
+      </c>
+      <c r="M15" s="5">
+        <v>5</v>
+      </c>
+      <c r="N15" t="s">
+        <v>51</v>
+      </c>
+      <c r="O15">
+        <v>6</v>
+      </c>
+      <c r="P15">
+        <v>11</v>
+      </c>
+      <c r="Q15" s="17">
+        <f t="shared" si="0"/>
+        <v>0.36666666666666664</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>33</v>
+      </c>
+      <c r="H16" s="1">
+        <v>28572</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
+        <v>10</v>
+      </c>
+      <c r="L16" s="5">
+        <v>25</v>
+      </c>
+      <c r="M16" s="5">
+        <v>-15</v>
+      </c>
+      <c r="N16" t="s">
+        <v>52</v>
+      </c>
+      <c r="O16">
+        <v>30</v>
+      </c>
+      <c r="P16">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17" s="1">
+        <v>36130</v>
+      </c>
+      <c r="I17" s="5">
+        <v>2</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="K17" s="5">
+        <v>18</v>
+      </c>
+      <c r="L17" s="5">
+        <v>21</v>
+      </c>
+      <c r="M17" s="5">
+        <v>-3</v>
+      </c>
+      <c r="N17" t="s">
+        <v>51</v>
+      </c>
+      <c r="O17">
+        <v>22</v>
+      </c>
+      <c r="P17">
+        <v>23</v>
+      </c>
+      <c r="Q17" s="17">
+        <f t="shared" si="0"/>
+        <v>0.76666666666666672</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1">
+        <v>33018</v>
+      </c>
+      <c r="I18" s="5">
+        <v>3</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K18" s="5">
+        <v>22</v>
+      </c>
+      <c r="L18" s="5">
+        <v>18</v>
+      </c>
+      <c r="M18" s="5">
+        <v>4</v>
+      </c>
+      <c r="N18" t="s">
+        <v>51</v>
+      </c>
+      <c r="O18">
+        <v>7</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="17">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="H19" s="1">
+        <v>36310</v>
+      </c>
+      <c r="I19" s="5">
+        <v>3</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K19" s="5">
+        <v>20</v>
+      </c>
+      <c r="L19" s="5">
+        <v>16</v>
+      </c>
+      <c r="M19" s="5">
+        <v>4</v>
+      </c>
+      <c r="N19" t="s">
+        <v>51</v>
+      </c>
+      <c r="O19">
+        <v>9</v>
+      </c>
+      <c r="P19">
+        <v>12</v>
+      </c>
+      <c r="Q19" s="17">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>16</v>
+      </c>
+      <c r="H20" s="1">
+        <v>37444</v>
+      </c>
+      <c r="I20" s="5">
+        <v>2</v>
+      </c>
+      <c r="J20" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="K20" s="5">
+        <v>18</v>
+      </c>
+      <c r="L20" s="5">
+        <v>22</v>
+      </c>
+      <c r="M20" s="5">
+        <v>-4</v>
+      </c>
+      <c r="N20" t="s">
+        <v>51</v>
+      </c>
+      <c r="O20">
+        <v>23</v>
+      </c>
+      <c r="P20">
+        <v>16</v>
+      </c>
+      <c r="Q20" s="17">
+        <f t="shared" si="0"/>
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>33</v>
+      </c>
+      <c r="H21" s="1">
+        <v>36481</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1</v>
+      </c>
+      <c r="J21" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="K21" s="5">
+        <v>18</v>
+      </c>
+      <c r="L21" s="5">
+        <v>24</v>
+      </c>
+      <c r="M21" s="5">
+        <v>-6</v>
+      </c>
+      <c r="N21" t="s">
+        <v>52</v>
+      </c>
+      <c r="O21">
+        <v>27</v>
+      </c>
+      <c r="P21">
+        <v>27</v>
+      </c>
+      <c r="Q21" s="17">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22" s="1">
+        <v>36325</v>
+      </c>
+      <c r="I22" s="5">
+        <v>5</v>
+      </c>
+      <c r="J22" s="5">
+        <v>1</v>
+      </c>
+      <c r="K22" s="5">
+        <v>25</v>
+      </c>
+      <c r="L22" s="5">
+        <v>8</v>
+      </c>
+      <c r="M22" s="5">
+        <v>17</v>
+      </c>
+      <c r="N22" t="s">
+        <v>51</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>9</v>
+      </c>
+      <c r="Q22" s="17">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>25</v>
+      </c>
+      <c r="H23" s="1">
+        <v>36380</v>
+      </c>
+      <c r="I23" s="5">
+        <v>2</v>
+      </c>
+      <c r="J23" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="K23" s="5">
+        <v>19</v>
+      </c>
+      <c r="L23" s="5">
+        <v>21</v>
+      </c>
+      <c r="M23" s="5">
+        <v>-2</v>
+      </c>
+      <c r="N23" t="s">
+        <v>51</v>
+      </c>
+      <c r="O23">
+        <v>20</v>
+      </c>
+      <c r="P23">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="17">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>25</v>
+      </c>
+      <c r="H24" s="1">
+        <v>27557</v>
+      </c>
+      <c r="I24" s="5">
+        <v>3</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K24" s="5">
+        <v>19</v>
+      </c>
+      <c r="L24" s="5">
+        <v>20</v>
+      </c>
+      <c r="M24" s="5">
+        <v>-1</v>
+      </c>
+      <c r="N24" t="s">
+        <v>51</v>
+      </c>
+      <c r="O24">
+        <v>17</v>
+      </c>
+      <c r="P24">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="17">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>9</v>
+      </c>
+      <c r="H25" s="1">
+        <v>34911</v>
+      </c>
+      <c r="I25" s="5">
+        <v>3</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K25" s="5">
+        <v>20</v>
+      </c>
+      <c r="L25" s="5">
+        <v>21</v>
+      </c>
+      <c r="M25" s="5">
+        <v>-1</v>
+      </c>
+      <c r="N25" t="s">
+        <v>51</v>
+      </c>
+      <c r="O25">
+        <v>15</v>
+      </c>
+      <c r="P25">
+        <v>14</v>
+      </c>
+      <c r="Q25" s="17">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>11</v>
+      </c>
+      <c r="H26" s="1">
+        <v>35707</v>
+      </c>
+      <c r="I26" s="5">
+        <v>2</v>
+      </c>
+      <c r="J26" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="K26" s="5">
+        <v>18</v>
+      </c>
+      <c r="L26" s="5">
+        <v>17</v>
+      </c>
+      <c r="M26" s="5">
+        <v>1</v>
+      </c>
+      <c r="N26" t="s">
+        <v>51</v>
+      </c>
+      <c r="O26">
+        <v>19</v>
+      </c>
+      <c r="P26">
+        <v>15</v>
+      </c>
+      <c r="Q26" s="17">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="H27" s="1">
+        <v>36429</v>
+      </c>
+      <c r="I27" s="5">
+        <v>3</v>
+      </c>
+      <c r="J27" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K27" s="5">
+        <v>21</v>
+      </c>
+      <c r="L27" s="5">
+        <v>19</v>
+      </c>
+      <c r="M27" s="5">
+        <v>2</v>
+      </c>
+      <c r="N27" t="s">
+        <v>51</v>
+      </c>
+      <c r="O27">
+        <v>12</v>
+      </c>
+      <c r="P27">
+        <v>8</v>
+      </c>
+      <c r="Q27" s="17">
+        <f t="shared" si="0"/>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>19</v>
+      </c>
+      <c r="H28" s="1">
+        <v>28491</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28" s="5">
+        <v>0</v>
+      </c>
+      <c r="K28" s="5">
+        <v>17</v>
+      </c>
+      <c r="L28" s="5">
+        <v>25</v>
+      </c>
+      <c r="M28" s="5">
+        <v>-8</v>
+      </c>
+      <c r="N28" t="s">
+        <v>52</v>
+      </c>
+      <c r="O28">
+        <v>28</v>
+      </c>
+      <c r="P28">
+        <v>28</v>
+      </c>
+      <c r="Q28" s="17">
+        <f t="shared" si="0"/>
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>17</v>
+      </c>
+      <c r="H29" s="1">
+        <v>32792</v>
+      </c>
+      <c r="I29" s="5">
+        <v>2</v>
+      </c>
+      <c r="J29" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="K29" s="5">
+        <v>15</v>
+      </c>
+      <c r="L29" s="5">
+        <v>20</v>
+      </c>
+      <c r="M29" s="5">
+        <v>-5</v>
+      </c>
+      <c r="N29" t="s">
+        <v>51</v>
+      </c>
+      <c r="O29">
+        <v>24</v>
+      </c>
+      <c r="P29">
+        <v>24</v>
+      </c>
+      <c r="Q29" s="17">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30">
+        <v>24</v>
+      </c>
+      <c r="H30" s="1">
+        <v>37171</v>
+      </c>
+      <c r="I30" s="5">
+        <v>2</v>
+      </c>
+      <c r="J30" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="K30" s="5">
+        <v>21</v>
+      </c>
+      <c r="L30" s="5">
+        <v>15</v>
+      </c>
+      <c r="M30" s="5">
+        <v>6</v>
+      </c>
+      <c r="N30" t="s">
+        <v>51</v>
+      </c>
+      <c r="O30">
+        <v>18</v>
+      </c>
+      <c r="P30">
+        <v>20</v>
+      </c>
+      <c r="Q30" s="17">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>25</v>
+      </c>
+      <c r="H31" s="1">
+        <v>37441</v>
+      </c>
+      <c r="I31" s="5">
+        <v>3</v>
+      </c>
+      <c r="J31" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="K31" s="5">
+        <v>20</v>
+      </c>
+      <c r="L31" s="5">
+        <v>21</v>
+      </c>
+      <c r="M31" s="5">
+        <v>-1</v>
+      </c>
+      <c r="N31" t="s">
+        <v>51</v>
+      </c>
+      <c r="O31">
+        <v>15</v>
+      </c>
+      <c r="P31">
+        <v>19</v>
+      </c>
+      <c r="Q31" s="17">
+        <f t="shared" si="0"/>
+        <v>0.6333333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:Q1" xr:uid="{009EEB42-AF0B-4CD6-B9D9-CB19FB8E0451}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="B1" sqref="B1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1336,18 +3039,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F31">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9A8189-CEEB-4B9A-8A98-7023554FFA86}">
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A25:J26"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1401,34 +3108,34 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F2" s="5">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="G2" s="5">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H2" s="5">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="I2" s="5">
-        <v>17</v>
+        <v>-7</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K2" s="1">
         <v>43610</v>
@@ -1524,31 +3231,31 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="5">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="G5" s="5">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H5" s="5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J5" t="s">
         <v>51</v>
@@ -1565,10 +3272,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1583,13 +3290,13 @@
         <v>0.6</v>
       </c>
       <c r="G6" s="5">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H6" s="5">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J6" t="s">
         <v>51</v>
@@ -1606,31 +3313,31 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" s="5">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="G7" s="5">
+        <v>15</v>
+      </c>
+      <c r="H7" s="5">
         <v>20</v>
       </c>
-      <c r="H7" s="5">
-        <v>15</v>
-      </c>
       <c r="I7" s="5">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="J7" t="s">
         <v>51</v>
@@ -1647,13 +3354,13 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -1668,10 +3375,10 @@
         <v>22</v>
       </c>
       <c r="H8" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I8" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J8" t="s">
         <v>51</v>
@@ -1688,10 +3395,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -1706,13 +3413,13 @@
         <v>0.6</v>
       </c>
       <c r="G9" s="5">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H9" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I9" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J9" t="s">
         <v>51</v>
@@ -1729,34 +3436,34 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F10" s="5">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G10" s="5">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H10" s="5">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I10" s="5">
-        <v>4</v>
+        <v>-9</v>
       </c>
       <c r="J10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K10" s="1">
         <v>43610</v>
@@ -1770,13 +3477,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -1788,13 +3495,13 @@
         <v>0.6</v>
       </c>
       <c r="G11" s="5">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H11" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I11" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J11" t="s">
         <v>51</v>
@@ -1811,31 +3518,31 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" s="5">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="G12" s="5">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H12" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I12" s="5">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="J12" t="s">
         <v>51</v>
@@ -1852,31 +3559,31 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="5">
+        <v>4</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="G13" s="5">
+        <v>23</v>
+      </c>
+      <c r="H13" s="5">
+        <v>20</v>
+      </c>
+      <c r="I13" s="5">
         <v>3</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="G13" s="5">
-        <v>21</v>
-      </c>
-      <c r="H13" s="5">
-        <v>19</v>
-      </c>
-      <c r="I13" s="5">
-        <v>2</v>
       </c>
       <c r="J13" t="s">
         <v>51</v>
@@ -1893,10 +3600,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1911,13 +3618,13 @@
         <v>0.6</v>
       </c>
       <c r="G14" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H14" s="5">
         <v>19</v>
       </c>
       <c r="I14" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J14" t="s">
         <v>51</v>
@@ -1934,13 +3641,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
@@ -1955,10 +3662,10 @@
         <v>20</v>
       </c>
       <c r="H15" s="5">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I15" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J15" t="s">
         <v>51</v>
@@ -1975,34 +3682,34 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F16" s="5">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G16" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H16" s="5">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I16" s="5">
-        <v>-1</v>
+        <v>-15</v>
       </c>
       <c r="J16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K16" s="1">
         <v>43610</v>
@@ -2016,31 +3723,31 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" s="5">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="G17" s="5">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H17" s="5">
         <v>21</v>
       </c>
       <c r="I17" s="5">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="J17" t="s">
         <v>51</v>
@@ -2057,13 +3764,13 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
@@ -2075,13 +3782,13 @@
         <v>0.6</v>
       </c>
       <c r="G18" s="5">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H18" s="5">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I18" s="5">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="J18" t="s">
         <v>51</v>
@@ -2098,10 +3805,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -2110,19 +3817,19 @@
         <v>6</v>
       </c>
       <c r="E19" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" s="5">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="G19" s="5">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H19" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I19" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J19" t="s">
         <v>51</v>
@@ -2139,13 +3846,13 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -2160,10 +3867,10 @@
         <v>18</v>
       </c>
       <c r="H20" s="5">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I20" s="5">
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="J20" t="s">
         <v>51</v>
@@ -2180,34 +3887,34 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="G21" s="5">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="5">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I21" s="5">
-        <v>-2</v>
+        <v>-6</v>
       </c>
       <c r="J21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K21" s="1">
         <v>43610</v>
@@ -2221,31 +3928,31 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F22" s="5">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="G22" s="5">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H22" s="5">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="I22" s="5">
-        <v>-2</v>
+        <v>17</v>
       </c>
       <c r="J22" t="s">
         <v>51</v>
@@ -2262,13 +3969,13 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -2280,13 +3987,13 @@
         <v>0.4</v>
       </c>
       <c r="G23" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H23" s="5">
         <v>21</v>
       </c>
       <c r="I23" s="5">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="J23" t="s">
         <v>51</v>
@@ -2303,31 +4010,31 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="5">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="G24" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H24" s="5">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I24" s="5">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="J24" t="s">
         <v>51</v>
@@ -2344,10 +4051,10 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
         <v>36</v>
@@ -2356,19 +4063,19 @@
         <v>6</v>
       </c>
       <c r="E25" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F25" s="5">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="G25" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H25" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I25" s="5">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="J25" t="s">
         <v>51</v>
@@ -2385,13 +4092,13 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -2403,13 +4110,13 @@
         <v>0.4</v>
       </c>
       <c r="G26" s="5">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H26" s="5">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I26" s="5">
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="J26" t="s">
         <v>51</v>
@@ -2426,34 +4133,34 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="5">
+        <v>3</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="G27" s="5">
+        <v>21</v>
+      </c>
+      <c r="H27" s="5">
+        <v>19</v>
+      </c>
+      <c r="I27" s="5">
         <v>2</v>
       </c>
-      <c r="F27" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="G27" s="5">
-        <v>16</v>
-      </c>
-      <c r="H27" s="5">
-        <v>23</v>
-      </c>
-      <c r="I27" s="5">
-        <v>-7</v>
-      </c>
       <c r="J27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K27" s="1">
         <v>43610</v>
@@ -2467,31 +4174,31 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" s="5">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G28" s="5">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H28" s="5">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I28" s="5">
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="J28" t="s">
         <v>52</v>
@@ -2508,34 +4215,34 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F29" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G29" s="5">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H29" s="5">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I29" s="5">
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="J29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K29" s="1">
         <v>43610</v>
@@ -2549,34 +4256,34 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G30" s="5">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H30" s="5">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I30" s="5">
-        <v>-9</v>
+        <v>6</v>
       </c>
       <c r="J30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K30" s="1">
         <v>43610</v>
@@ -2590,34 +4297,34 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F31" s="5">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="G31" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H31" s="5">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I31" s="5">
-        <v>-15</v>
+        <v>-1</v>
       </c>
       <c r="J31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K31" s="1">
         <v>43610</v>
@@ -2630,18 +4337,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{4E9A8189-CEEB-4B9A-8A98-7023554FFA86}"/>
+  <autoFilter ref="A1:M1" xr:uid="{4E9A8189-CEEB-4B9A-8A98-7023554FFA86}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M31">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A681623-D911-44C6-8EF5-3A2224EF243B}">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H1" sqref="F1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2680,19 +4391,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="1">
-        <v>33018</v>
+        <v>37414</v>
       </c>
       <c r="F2" s="1">
         <v>43610</v>
@@ -2706,19 +4417,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="1">
-        <v>34628</v>
+        <v>37371</v>
       </c>
       <c r="F3" s="1">
         <v>43610</v>
@@ -2758,19 +4469,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="1">
-        <v>27557</v>
+        <v>29490</v>
       </c>
       <c r="F5" s="1">
         <v>43610</v>
@@ -2784,10 +4495,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -2796,7 +4507,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="1">
-        <v>37371</v>
+        <v>37189</v>
       </c>
       <c r="F6" s="1">
         <v>43610</v>
@@ -2810,10 +4521,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -2822,7 +4533,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="1">
-        <v>37189</v>
+        <v>37903</v>
       </c>
       <c r="F7" s="1">
         <v>43610</v>
@@ -2862,19 +4573,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="1">
-        <v>36429</v>
+        <v>33010</v>
       </c>
       <c r="F9" s="1">
         <v>43610</v>
@@ -2888,19 +4599,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="1">
-        <v>36325</v>
+        <v>33437</v>
       </c>
       <c r="F10" s="1">
         <v>43610</v>
@@ -2914,10 +4625,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -2926,7 +4637,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="1">
-        <v>33010</v>
+        <v>37934</v>
       </c>
       <c r="F11" s="1">
         <v>43610</v>
@@ -2940,19 +4651,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="1">
-        <v>36590</v>
+        <v>35537</v>
       </c>
       <c r="F12" s="1">
         <v>43610</v>
@@ -2966,19 +4677,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="1">
-        <v>36310</v>
+        <v>34628</v>
       </c>
       <c r="F13" s="1">
         <v>43610</v>
@@ -2992,10 +4703,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -3004,7 +4715,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="1">
-        <v>29490</v>
+        <v>36590</v>
       </c>
       <c r="F14" s="1">
         <v>43610</v>
@@ -3018,19 +4729,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="1">
-        <v>34911</v>
+        <v>36590</v>
       </c>
       <c r="F15" s="1">
         <v>43610</v>
@@ -3044,19 +4755,19 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="1">
-        <v>35707</v>
+        <v>28572</v>
       </c>
       <c r="F16" s="1">
         <v>43610</v>
@@ -3070,10 +4781,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -3082,7 +4793,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="1">
-        <v>37444</v>
+        <v>36130</v>
       </c>
       <c r="F17" s="1">
         <v>43610</v>
@@ -3096,19 +4807,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="1">
-        <v>36590</v>
+        <v>33018</v>
       </c>
       <c r="F18" s="1">
         <v>43610</v>
@@ -3122,10 +4833,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -3134,7 +4845,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="1">
-        <v>37934</v>
+        <v>36310</v>
       </c>
       <c r="F19" s="1">
         <v>43610</v>
@@ -3148,19 +4859,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="1">
-        <v>37441</v>
+        <v>37444</v>
       </c>
       <c r="F20" s="1">
         <v>43610</v>
@@ -3174,19 +4885,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="1">
-        <v>37171</v>
+        <v>36481</v>
       </c>
       <c r="F21" s="1">
         <v>43610</v>
@@ -3200,19 +4911,19 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="1">
-        <v>36380</v>
+        <v>36325</v>
       </c>
       <c r="F22" s="1">
         <v>43610</v>
@@ -3226,19 +4937,19 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="1">
-        <v>35537</v>
+        <v>36380</v>
       </c>
       <c r="F23" s="1">
         <v>43610</v>
@@ -3252,19 +4963,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="1">
-        <v>36130</v>
+        <v>27557</v>
       </c>
       <c r="F24" s="1">
         <v>43610</v>
@@ -3278,10 +4989,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
         <v>36</v>
@@ -3290,7 +5001,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="1">
-        <v>32792</v>
+        <v>34911</v>
       </c>
       <c r="F25" s="1">
         <v>43610</v>
@@ -3304,19 +5015,19 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="1">
-        <v>37903</v>
+        <v>35707</v>
       </c>
       <c r="F26" s="1">
         <v>43610</v>
@@ -3330,19 +5041,19 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="1">
-        <v>37414</v>
+        <v>36429</v>
       </c>
       <c r="F27" s="1">
         <v>43610</v>
@@ -3356,19 +5067,19 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="1">
-        <v>36481</v>
+        <v>28491</v>
       </c>
       <c r="F28" s="1">
         <v>43610</v>
@@ -3382,19 +5093,19 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="1">
-        <v>28491</v>
+        <v>32792</v>
       </c>
       <c r="F29" s="1">
         <v>43610</v>
@@ -3408,19 +5119,19 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="1">
-        <v>33437</v>
+        <v>37171</v>
       </c>
       <c r="F30" s="1">
         <v>43610</v>
@@ -3434,19 +5145,19 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="1">
-        <v>28572</v>
+        <v>37441</v>
       </c>
       <c r="F31" s="1">
         <v>43610</v>
@@ -3459,13 +5170,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{1A681623-D911-44C6-8EF5-3A2224EF243B}"/>
+  <autoFilter ref="A1:H1" xr:uid="{1A681623-D911-44C6-8EF5-3A2224EF243B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H31">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0031D708-A1F7-44B9-81EF-301B8BD736BE}">
   <dimension ref="A1:K152"/>
   <sheetViews>
@@ -8779,11 +10494,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153748E9-27BB-4A14-A27E-1E1210878F64}">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>

</xml_diff>